<commit_message>
Ignore generated images and extracted outputs
</commit_message>
<xml_diff>
--- a/Qwen_Results.xlsx
+++ b/Qwen_Results.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>حلىمى علي ريان</t>
+          <t>طلمي علي ريان</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>حسين محمد ماهر براء الدين</t>
+          <t>حسين محمد ماهر بهاء الدين</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>محمد منير عبد الحميد كمال</t>
+          <t>محمد مزير عبد الحميد كمال</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>عمرو أيهاب مختار قرخات</t>
+          <t>عدو ايها ب مختار قرحات</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>محمد عبد الرحيم سالم عبد الهادي</t>
+          <t>محمد عبد الرحيم سالم عبداللهي</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>زياد ايهاه محمد ممدوح ناقع</t>
+          <t>زياد ايهاهاب محمد ممدوح ناقع</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>اية احمد محمد خشبه</t>
+          <t>اية احمد محمد خشيمه</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>جنى ايمن وقائى محمد عيسى</t>
+          <t>جنى ايمن وفأى محمد عيسى</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>سلمى محمد ابراهيم قتحدى ابوريدة</t>
+          <t>سلمى محمد ابراهيم قتحى ابو ريده</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>مروان عمرو عبد المجيد فؤاد احمد شكرى</t>
+          <t>مروان عمرو عبد المجيد قواد احمد شكرى</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>جمانة عمرو مصطفى عبد الصالح عرابي</t>
+          <t>جمانة عمرو مصطفى عبد الصالح عرايبي</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>حمزة احمد محمد منير الجوهري</t>
+          <t>حمزة احمد محمد مثير الجوهري</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Ignore generated images and extracted outputs"
This reverts commit 37b2cf8f99add1624eb64d592668c7c217908da1.
</commit_message>
<xml_diff>
--- a/Qwen_Results.xlsx
+++ b/Qwen_Results.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>طلمي علي ريان</t>
+          <t>حلىمى علي ريان</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>حسين محمد ماهر بهاء الدين</t>
+          <t>حسين محمد ماهر براء الدين</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>محمد مزير عبد الحميد كمال</t>
+          <t>محمد منير عبد الحميد كمال</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>عدو ايها ب مختار قرحات</t>
+          <t>عمرو أيهاب مختار قرخات</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>محمد عبد الرحيم سالم عبداللهي</t>
+          <t>محمد عبد الرحيم سالم عبد الهادي</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>زياد ايهاهاب محمد ممدوح ناقع</t>
+          <t>زياد ايهاه محمد ممدوح ناقع</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>اية احمد محمد خشيمه</t>
+          <t>اية احمد محمد خشبه</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>جنى ايمن وفأى محمد عيسى</t>
+          <t>جنى ايمن وقائى محمد عيسى</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>سلمى محمد ابراهيم قتحى ابو ريده</t>
+          <t>سلمى محمد ابراهيم قتحدى ابوريدة</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>مروان عمرو عبد المجيد قواد احمد شكرى</t>
+          <t>مروان عمرو عبد المجيد فؤاد احمد شكرى</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>جمانة عمرو مصطفى عبد الصالح عرايبي</t>
+          <t>جمانة عمرو مصطفى عبد الصالح عرابي</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>حمزة احمد محمد مثير الجوهري</t>
+          <t>حمزة احمد محمد منير الجوهري</t>
         </is>
       </c>
     </row>

</xml_diff>